<commit_message>
chore: mise à jour des objectifs et actions du référentiel
</commit_message>
<xml_diff>
--- a/referentiel.xlsx
+++ b/referentiel.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="182">
   <si>
     <t xml:space="preserve">Theme</t>
   </si>
@@ -338,6 +338,234 @@
   </si>
   <si>
     <t xml:space="preserve">Problème déclaré ne permettant pas de reprendre une activité professionnelle immédiate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OBJECTIF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recherche de mode de garde</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trouver des solutions de garde d’enfant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Devenir aidant familial salarié</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obtenir le statut d’aidant familial </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rompre l’isolement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faire face à la prise en charge d’une personne dépendante</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surmonter des difficultés éducatives ou de parentalité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faire face à un conflit familial et/ou une séparation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Travailler l’accès à une prestation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bénéficier d’un appui aux démarches administratives</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Travailler l’accès à la citoyenneté</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bénéficier d'un accompagnement à l'accès à la citoyenneté</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Travailler l’accès aux droits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bénéficier d’un accompagnement pour accéder aux droits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accompagnement dans les démarches numériques</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maitriser les fondamentaux du numérique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mise en place d'une mesure d'accompagnement adapté</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bénéficier d'une mesure d'accompagnement adapté</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prendre en compte une problématique judiciaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connaitre les voies de recours face à une discrimination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Réduire / apurer les dettes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faire face à une situation d'endettement / surendettement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Améliorer la gestion budgétaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Améliorer sa gestion budgétaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acquérir une autonomie budgétaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mettre en place une mesure de protection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mettre en place une mesure de protection financières (tutelles, curatelles, …)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faire une demande de droits sociaux ( RSA, ASS… )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rupture effective d'hébergemnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remonter dans les Situation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accèder au logement social</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accéder à un logement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S'informer sur les démarches liées au logement ( budget, état des lieux… )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S'informer sur les démarches liées au logement (budget, état des lieux… )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se maintenir dans le logement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changer de logement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Réduire les impayés</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Réduire les impayés de loyer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rechercher un hébergement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rechercher une solution d’hébergement temporaire </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se maintenir dans un hébergement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recherche d'un hébergement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Démarche de relogement suite à une problématique d'insalubrité ( DALO )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Améliorer la maitrise du français</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apprendre / Améliorer ses capacités en français </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Améliorer les savoirs : à l’écriture et la lecture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apprendre / Améliorer ses capacités en calcul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accéder à un véhicule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bénéficier d'un accompagnement permettant d'accèder à la mobilité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faire un point complet sur sa mobilité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bénéficier d'une aide financière pour le passage du permis de conduire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">action</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avoir accès aux transports en commun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trouver une solution de transport (hors acquisition ou entretien de véhicule)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bénéficier d'une aide financière pour l'achat de véhicule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obtenir le permis de conduire / code de la route</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obtenir le permis de conduire (code / conduite)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entretenir ou réparer son véhicule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Travailler la mobilité psychologique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Travailler la mobilité psychologique </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accéder a des service en ligne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accéder à une connexion internet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accéder à un ordinateur, une tablette ou un smartphone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mise en place d’une mesure d’accompagnement adapté</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accéder aux droits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bénéficier d’un accompagnement pour accéder aux droits et/ou aux soins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Travailler sur les comportements de santé (dépendances, hygiène corporelle, dépistage… )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Travailler sur les comportements de santé (dépendances, hygiène corporelle, dépistage, …)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accéder aux soins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mettre en place une mesure de protection administrative ou juridique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">action de l'accès au droit santé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faire une demande de droits sociaux (RSA, ASS, Prime d'activité, …)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Réalisation d'une demande de mesure de protection administrative ou juridique"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Constitution d’une demande d'aide financière pour l’achat d’un véhicule</t>
   </si>
 </sst>
 </file>
@@ -348,7 +576,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -382,8 +610,21 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -394,6 +635,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -487,7 +734,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -585,6 +832,22 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -605,10 +868,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:E121"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A38" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C120" activeCellId="0" sqref="C120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.35546875" defaultRowHeight="13.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -617,7 +880,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="57.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="40.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="40.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1669,6 +1932,824 @@
       <c r="D67" s="10"/>
       <c r="E67" s="8" t="s">
         <v>105</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E77" s="25" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="85" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B85" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="C85" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="D85" s="26"/>
+      <c r="E85" s="26"/>
+    </row>
+    <row r="86" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B86" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="C86" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="D86" s="26"/>
+      <c r="E86" s="26" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="102" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="B102" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="C102" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="D102" s="26"/>
+      <c r="E102" s="26" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="104" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="B104" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="C104" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="D104" s="26"/>
+      <c r="E104" s="26" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="116" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="B116" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="C116" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="D116" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E116" s="26" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E117" s="28" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B118" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B119" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B120" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B121" s="1" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Mise à jour des actions et des objectifs
</commit_message>
<xml_diff>
--- a/referentiel.xlsx
+++ b/referentiel.xlsx
@@ -10,6 +10,9 @@
   <sheets>
     <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Sheet 1'!$A$1:$E$119</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="182">
   <si>
     <t xml:space="preserve">Theme</t>
   </si>
@@ -136,7 +139,7 @@
     <t xml:space="preserve">Ressources précaires</t>
   </si>
   <si>
-    <t xml:space="preserve">Ressources précaires (inférieur au seuil de pauvreté)</t>
+    <t xml:space="preserve">Ressources précaires (inférieures au seuil de pauvreté)</t>
   </si>
   <si>
     <t xml:space="preserve">Besoin d'un soutien alimentaire</t>
@@ -304,7 +307,7 @@
     <t xml:space="preserve">Accès ou utilisation difficile des outils numériques</t>
   </si>
   <si>
-    <t xml:space="preserve">Usage basic du numérique (-50%)</t>
+    <t xml:space="preserve">Usage basique du numérique (-50%)</t>
   </si>
   <si>
     <t xml:space="preserve">Non maitrise du numérique (0%)</t>
@@ -400,7 +403,7 @@
     <t xml:space="preserve">Prendre en compte une problématique judiciaire</t>
   </si>
   <si>
-    <t xml:space="preserve">Connaitre les voies de recours face à une discrimination</t>
+    <t xml:space="preserve">Connaître les voies de recours face à une discrimination</t>
   </si>
   <si>
     <t xml:space="preserve">Réduire / apurer les dettes</t>
@@ -615,6 +618,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -843,11 +847,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -860,18 +864,53 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E121"/>
+  <dimension ref="A1:E122"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A38" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C120" activeCellId="0" sqref="C120"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E119" activeCellId="0" sqref="E119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.35546875" defaultRowHeight="13.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -880,7 +919,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="57.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="40.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="40.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -900,7 +939,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -949,7 +988,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
         <v>5</v>
       </c>
@@ -964,7 +1003,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
         <v>5</v>
       </c>
@@ -979,7 +1018,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
         <v>5</v>
       </c>
@@ -1043,7 +1082,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
         <v>16</v>
       </c>
@@ -1058,7 +1097,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
         <v>16</v>
       </c>
@@ -1088,7 +1127,7 @@
       </c>
       <c r="E13" s="19"/>
     </row>
-    <row r="14" customFormat="false" ht="13.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.3" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="s">
         <v>16</v>
       </c>
@@ -1103,7 +1142,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.3" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="9" t="s">
         <v>16</v>
       </c>
@@ -1135,7 +1174,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="s">
         <v>32</v>
       </c>
@@ -1150,7 +1189,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="s">
         <v>32</v>
       </c>
@@ -1165,7 +1204,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="9" t="s">
         <v>32</v>
       </c>
@@ -1180,7 +1219,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="s">
         <v>32</v>
       </c>
@@ -1212,7 +1251,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
         <v>32</v>
       </c>
@@ -1244,7 +1283,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
         <v>40</v>
       </c>
@@ -1259,7 +1298,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="s">
         <v>40</v>
       </c>
@@ -1274,7 +1313,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="s">
         <v>40</v>
       </c>
@@ -1289,7 +1328,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="9" t="s">
         <v>40</v>
       </c>
@@ -1338,7 +1377,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="s">
         <v>40</v>
       </c>
@@ -1353,7 +1392,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="9" t="s">
         <v>40</v>
       </c>
@@ -1402,7 +1441,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="9" t="s">
         <v>40</v>
       </c>
@@ -1417,7 +1456,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="9" t="s">
         <v>40</v>
       </c>
@@ -1530,7 +1569,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="9" t="s">
         <v>69</v>
       </c>
@@ -1545,7 +1584,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="9" t="s">
         <v>69</v>
       </c>
@@ -1560,7 +1599,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="9" t="s">
         <v>69</v>
       </c>
@@ -1592,7 +1631,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="9" t="s">
         <v>69</v>
       </c>
@@ -1607,7 +1646,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="9" t="s">
         <v>69</v>
       </c>
@@ -1656,7 +1695,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="9" t="s">
         <v>69</v>
       </c>
@@ -1671,7 +1710,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="9" t="s">
         <v>69</v>
       </c>
@@ -1827,7 +1866,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="9" t="s">
         <v>98</v>
       </c>
@@ -1859,7 +1898,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="9" t="s">
         <v>98</v>
       </c>
@@ -1874,7 +1913,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="9" t="s">
         <v>98</v>
       </c>
@@ -1889,7 +1928,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="9" t="s">
         <v>98</v>
       </c>
@@ -1904,7 +1943,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="9" t="s">
         <v>98</v>
       </c>
@@ -1919,7 +1958,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="9" t="s">
         <v>98</v>
       </c>
@@ -1968,7 +2007,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
         <v>5</v>
       </c>
@@ -2171,7 +2210,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
         <v>32</v>
       </c>
@@ -2212,7 +2251,9 @@
       <c r="C85" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="D85" s="26"/>
+      <c r="D85" s="26" t="s">
+        <v>21</v>
+      </c>
       <c r="E85" s="26"/>
     </row>
     <row r="86" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2225,7 +2266,9 @@
       <c r="C86" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="D86" s="26"/>
+      <c r="D86" s="26" t="s">
+        <v>21</v>
+      </c>
       <c r="E86" s="26" t="s">
         <v>136</v>
       </c>
@@ -2247,7 +2290,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
         <v>40</v>
       </c>
@@ -2261,7 +2304,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
         <v>40</v>
       </c>
@@ -2275,7 +2318,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
         <v>40</v>
       </c>
@@ -2289,7 +2332,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
         <v>40</v>
       </c>
@@ -2388,7 +2431,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
         <v>61</v>
       </c>
@@ -2433,7 +2476,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
         <v>69</v>
       </c>
@@ -2474,7 +2517,9 @@
       <c r="C102" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="D102" s="26"/>
+      <c r="D102" s="26" t="s">
+        <v>21</v>
+      </c>
       <c r="E102" s="26" t="s">
         <v>158</v>
       </c>
@@ -2506,7 +2551,9 @@
       <c r="C104" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="D104" s="26"/>
+      <c r="D104" s="26" t="s">
+        <v>21</v>
+      </c>
       <c r="E104" s="26" t="s">
         <v>158</v>
       </c>
@@ -2528,7 +2575,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
         <v>69</v>
       </c>
@@ -2742,17 +2789,20 @@
         <v>181</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B120" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B121" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <autoFilter ref="A1:E119">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="ajouter"/>
+        <filter val="fusionner"/>
+        <filter val="modifier"/>
+        <filter val="supprimer"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2760,5 +2810,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
chore: mise à jour du référentiel
</commit_message>
<xml_diff>
--- a/referentiel.xlsx
+++ b/referentiel.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="182">
   <si>
     <t xml:space="preserve">Theme</t>
   </si>
@@ -904,13 +904,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="true">
+  <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E122"/>
+  <dimension ref="A1:G122"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E119" activeCellId="0" sqref="E119"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B4" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.35546875" defaultRowHeight="13.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -939,7 +939,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -953,6 +953,10 @@
       <c r="E2" s="8" t="s">
         <v>7</v>
       </c>
+      <c r="G2" s="0" t="str">
+        <f aca="false">IF(C2=E2, "-", "modifier")</f>
+        <v>-</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
@@ -970,6 +974,10 @@
       <c r="E3" s="8" t="s">
         <v>10</v>
       </c>
+      <c r="G3" s="0" t="str">
+        <f aca="false">IF(C3=E3, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
@@ -987,8 +995,12 @@
       <c r="E4" s="8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G4" s="0" t="str">
+        <f aca="false">IF(C4=E4, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
         <v>5</v>
       </c>
@@ -1002,8 +1014,12 @@
       <c r="E5" s="8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G5" s="0" t="str">
+        <f aca="false">IF(C5=E5, "-", "modifier")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
         <v>5</v>
       </c>
@@ -1017,8 +1033,12 @@
       <c r="E6" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G6" s="0" t="str">
+        <f aca="false">IF(C6=E6, "-", "modifier")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
         <v>5</v>
       </c>
@@ -1032,6 +1052,10 @@
       <c r="E7" s="8" t="s">
         <v>15</v>
       </c>
+      <c r="G7" s="0" t="str">
+        <f aca="false">IF(C7=E7, "-", "modifier")</f>
+        <v>-</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="s">
@@ -1049,6 +1073,10 @@
       <c r="E8" s="15" t="s">
         <v>19</v>
       </c>
+      <c r="G8" s="0" t="str">
+        <f aca="false">IF(C8=E8, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
@@ -1064,6 +1092,10 @@
         <v>21</v>
       </c>
       <c r="E9" s="18"/>
+      <c r="G9" s="0" t="str">
+        <f aca="false">IF(C9=E9, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
@@ -1081,8 +1113,12 @@
       <c r="E10" s="8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G10" s="0" t="str">
+        <f aca="false">IF(C10=E10, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
         <v>16</v>
       </c>
@@ -1096,8 +1132,12 @@
       <c r="E11" s="8" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G11" s="0" t="str">
+        <f aca="false">IF(C11=E11, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
         <v>16</v>
       </c>
@@ -1111,6 +1151,10 @@
       <c r="E12" s="8" t="s">
         <v>26</v>
       </c>
+      <c r="G12" s="0" t="str">
+        <f aca="false">IF(C12=E12, "-", "modifier")</f>
+        <v>-</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="12" t="s">
@@ -1126,8 +1170,12 @@
         <v>21</v>
       </c>
       <c r="E13" s="19"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.3" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G13" s="0" t="str">
+        <f aca="false">IF(C13=E13, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="s">
         <v>16</v>
       </c>
@@ -1141,8 +1189,12 @@
       <c r="E14" s="20" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.3" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G14" s="0" t="str">
+        <f aca="false">IF(C14=E14, "-", "modifier")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="9" t="s">
         <v>16</v>
       </c>
@@ -1156,6 +1208,10 @@
       <c r="E15" s="8" t="s">
         <v>30</v>
       </c>
+      <c r="G15" s="0" t="str">
+        <f aca="false">IF(C15=E15, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="12" t="s">
@@ -1173,8 +1229,12 @@
       <c r="E16" s="15" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G16" s="0" t="str">
+        <f aca="false">IF(C16=E16, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="s">
         <v>32</v>
       </c>
@@ -1188,8 +1248,12 @@
       <c r="E17" s="8" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G17" s="0" t="str">
+        <f aca="false">IF(C17=E17, "-", "modifier")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="s">
         <v>32</v>
       </c>
@@ -1203,8 +1267,12 @@
       <c r="E18" s="8" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G18" s="0" t="str">
+        <f aca="false">IF(C18=E18, "-", "modifier")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="9" t="s">
         <v>32</v>
       </c>
@@ -1218,8 +1286,12 @@
       <c r="E19" s="8" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G19" s="0" t="str">
+        <f aca="false">IF(C19=E19, "-", "modifier")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="s">
         <v>32</v>
       </c>
@@ -1233,6 +1305,10 @@
       <c r="E20" s="8" t="s">
         <v>36</v>
       </c>
+      <c r="G20" s="0" t="str">
+        <f aca="false">IF(C20=E20, "-", "modifier")</f>
+        <v>-</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="s">
@@ -1250,8 +1326,12 @@
       <c r="E21" s="8" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G21" s="0" t="str">
+        <f aca="false">IF(C21=E21, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
         <v>32</v>
       </c>
@@ -1265,6 +1345,10 @@
       <c r="E22" s="8" t="s">
         <v>39</v>
       </c>
+      <c r="G22" s="0" t="str">
+        <f aca="false">IF(C22=E22, "-", "modifier")</f>
+        <v>-</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="s">
@@ -1282,8 +1366,12 @@
       <c r="E23" s="8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G23" s="0" t="str">
+        <f aca="false">IF(C23=E23, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
         <v>40</v>
       </c>
@@ -1297,8 +1385,12 @@
       <c r="E24" s="8" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G24" s="0" t="str">
+        <f aca="false">IF(C24=E24, "-", "modifier")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="s">
         <v>40</v>
       </c>
@@ -1312,8 +1404,12 @@
       <c r="E25" s="8" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G25" s="0" t="str">
+        <f aca="false">IF(C25=E25, "-", "modifier")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="s">
         <v>40</v>
       </c>
@@ -1327,8 +1423,12 @@
       <c r="E26" s="8" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G26" s="0" t="str">
+        <f aca="false">IF(C26=E26, "-", "modifier")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="9" t="s">
         <v>40</v>
       </c>
@@ -1342,6 +1442,10 @@
       <c r="E27" s="8" t="s">
         <v>46</v>
       </c>
+      <c r="G27" s="0" t="str">
+        <f aca="false">IF(C27=E27, "-", "modifier")</f>
+        <v>-</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="s">
@@ -1359,6 +1463,10 @@
       <c r="E28" s="8" t="s">
         <v>48</v>
       </c>
+      <c r="G28" s="0" t="str">
+        <f aca="false">IF(C28=E28, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="9" t="s">
@@ -1376,8 +1484,12 @@
       <c r="E29" s="8" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G29" s="0" t="str">
+        <f aca="false">IF(C29=E29, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="s">
         <v>40</v>
       </c>
@@ -1391,8 +1503,12 @@
       <c r="E30" s="8" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G30" s="0" t="str">
+        <f aca="false">IF(C30=E30, "-", "modifier")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="9" t="s">
         <v>40</v>
       </c>
@@ -1406,6 +1522,10 @@
       <c r="E31" s="8" t="s">
         <v>52</v>
       </c>
+      <c r="G31" s="0" t="str">
+        <f aca="false">IF(C31=E31, "-", "modifier")</f>
+        <v>-</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="9" t="s">
@@ -1423,6 +1543,10 @@
       <c r="E32" s="8" t="s">
         <v>54</v>
       </c>
+      <c r="G32" s="0" t="str">
+        <f aca="false">IF(C32=E32, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="9" t="s">
@@ -1440,8 +1564,12 @@
       <c r="E33" s="8" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G33" s="0" t="str">
+        <f aca="false">IF(C33=E33, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="9" t="s">
         <v>40</v>
       </c>
@@ -1455,8 +1583,12 @@
       <c r="E34" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G34" s="0" t="str">
+        <f aca="false">IF(C34=E34, "-", "modifier")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="9" t="s">
         <v>40</v>
       </c>
@@ -1470,6 +1602,10 @@
       <c r="E35" s="8" t="s">
         <v>58</v>
       </c>
+      <c r="G35" s="0" t="str">
+        <f aca="false">IF(C35=E35, "-", "modifier")</f>
+        <v>-</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="9" t="s">
@@ -1485,6 +1621,10 @@
       <c r="E36" s="8" t="s">
         <v>60</v>
       </c>
+      <c r="G36" s="0" t="str">
+        <f aca="false">IF(C36=E36, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="9" t="s">
@@ -1502,6 +1642,10 @@
       <c r="E37" s="8" t="s">
         <v>63</v>
       </c>
+      <c r="G37" s="0" t="str">
+        <f aca="false">IF(C37=E37, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="9" t="s">
@@ -1519,6 +1663,10 @@
       <c r="E38" s="8" t="s">
         <v>65</v>
       </c>
+      <c r="G38" s="0" t="str">
+        <f aca="false">IF(C38=E38, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="9" t="s">
@@ -1536,6 +1684,10 @@
       <c r="E39" s="8" t="s">
         <v>67</v>
       </c>
+      <c r="G39" s="0" t="str">
+        <f aca="false">IF(C39=E39, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="9" t="s">
@@ -1551,6 +1703,10 @@
       <c r="E40" s="8" t="s">
         <v>68</v>
       </c>
+      <c r="G40" s="0" t="str">
+        <f aca="false">IF(C40=E40, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="9" t="s">
@@ -1568,8 +1724,12 @@
       <c r="E41" s="8" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="42" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G41" s="0" t="str">
+        <f aca="false">IF(C41=E41, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="9" t="s">
         <v>69</v>
       </c>
@@ -1583,8 +1743,12 @@
       <c r="E42" s="8" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="43" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G42" s="0" t="str">
+        <f aca="false">IF(C42=E42, "-", "modifier")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="9" t="s">
         <v>69</v>
       </c>
@@ -1598,8 +1762,12 @@
       <c r="E43" s="23" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="44" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G43" s="0" t="str">
+        <f aca="false">IF(C43=E43, "-", "modifier")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="9" t="s">
         <v>69</v>
       </c>
@@ -1613,6 +1781,10 @@
       <c r="E44" s="8" t="s">
         <v>74</v>
       </c>
+      <c r="G44" s="0" t="str">
+        <f aca="false">IF(C44=E44, "-", "modifier")</f>
+        <v>-</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="9" t="s">
@@ -1630,8 +1802,12 @@
       <c r="E45" s="8" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="46" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G45" s="0" t="str">
+        <f aca="false">IF(C45=E45, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="9" t="s">
         <v>69</v>
       </c>
@@ -1645,8 +1821,12 @@
       <c r="E46" s="8" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="47" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G46" s="0" t="str">
+        <f aca="false">IF(C46=E46, "-", "modifier")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="9" t="s">
         <v>69</v>
       </c>
@@ -1660,6 +1840,10 @@
       <c r="E47" s="8" t="s">
         <v>78</v>
       </c>
+      <c r="G47" s="0" t="str">
+        <f aca="false">IF(C47=E47, "-", "modifier")</f>
+        <v>-</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="9" t="s">
@@ -1677,6 +1861,10 @@
       <c r="E48" s="8" t="s">
         <v>80</v>
       </c>
+      <c r="G48" s="0" t="str">
+        <f aca="false">IF(C48=E48, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="9" t="s">
@@ -1694,8 +1882,12 @@
       <c r="E49" s="8" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="50" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G49" s="0" t="str">
+        <f aca="false">IF(C49=E49, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="9" t="s">
         <v>69</v>
       </c>
@@ -1709,8 +1901,12 @@
       <c r="E50" s="8" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="51" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G50" s="0" t="str">
+        <f aca="false">IF(C50=E50, "-", "modifier")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="9" t="s">
         <v>69</v>
       </c>
@@ -1724,6 +1920,10 @@
       <c r="E51" s="8" t="s">
         <v>84</v>
       </c>
+      <c r="G51" s="0" t="str">
+        <f aca="false">IF(C51=E51, "-", "modifier")</f>
+        <v>-</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="9" t="s">
@@ -1739,6 +1939,10 @@
       <c r="E52" s="8" t="s">
         <v>85</v>
       </c>
+      <c r="G52" s="0" t="str">
+        <f aca="false">IF(C52=E52, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="9" t="s">
@@ -1754,6 +1958,10 @@
       <c r="E53" s="8" t="s">
         <v>86</v>
       </c>
+      <c r="G53" s="0" t="str">
+        <f aca="false">IF(C53=E53, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="9" t="s">
@@ -1771,6 +1979,10 @@
       <c r="E54" s="8" t="s">
         <v>89</v>
       </c>
+      <c r="G54" s="0" t="str">
+        <f aca="false">IF(C54=E54, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="9" t="s">
@@ -1786,6 +1998,10 @@
       <c r="E55" s="8" t="s">
         <v>90</v>
       </c>
+      <c r="G55" s="0" t="str">
+        <f aca="false">IF(C55=E55, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="9" t="s">
@@ -1803,6 +2019,10 @@
       <c r="E56" s="24" t="s">
         <v>92</v>
       </c>
+      <c r="G56" s="0" t="str">
+        <f aca="false">IF(C56=E56, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="9" t="s">
@@ -1820,6 +2040,10 @@
       <c r="E57" s="8" t="s">
         <v>94</v>
       </c>
+      <c r="G57" s="0" t="str">
+        <f aca="false">IF(C57=E57, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="9" t="s">
@@ -1835,6 +2059,10 @@
       <c r="E58" s="8" t="s">
         <v>95</v>
       </c>
+      <c r="G58" s="0" t="str">
+        <f aca="false">IF(C58=E58, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="9" t="s">
@@ -1850,6 +2078,10 @@
       <c r="E59" s="8" t="s">
         <v>96</v>
       </c>
+      <c r="G59" s="0" t="str">
+        <f aca="false">IF(C59=E59, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="9" t="s">
@@ -1865,8 +2097,12 @@
       <c r="E60" s="8" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="61" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G60" s="0" t="str">
+        <f aca="false">IF(C60=E60, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="9" t="s">
         <v>98</v>
       </c>
@@ -1880,6 +2116,10 @@
       <c r="E61" s="8" t="s">
         <v>99</v>
       </c>
+      <c r="G61" s="0" t="str">
+        <f aca="false">IF(C61=E61, "-", "modifier")</f>
+        <v>-</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="9" t="s">
@@ -1897,8 +2137,12 @@
       <c r="E62" s="8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="63" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G62" s="0" t="str">
+        <f aca="false">IF(C62=E62, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="9" t="s">
         <v>98</v>
       </c>
@@ -1912,8 +2156,12 @@
       <c r="E63" s="8" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="64" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G63" s="0" t="str">
+        <f aca="false">IF(C63=E63, "-", "modifier")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="9" t="s">
         <v>98</v>
       </c>
@@ -1927,8 +2175,12 @@
       <c r="E64" s="8" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="65" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G64" s="0" t="str">
+        <f aca="false">IF(C64=E64, "-", "modifier")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="9" t="s">
         <v>98</v>
       </c>
@@ -1942,8 +2194,12 @@
       <c r="E65" s="9" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="66" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G65" s="0" t="str">
+        <f aca="false">IF(C65=E65, "-", "modifier")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="9" t="s">
         <v>98</v>
       </c>
@@ -1957,8 +2213,12 @@
       <c r="E66" s="8" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="67" customFormat="false" ht="13.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G66" s="0" t="str">
+        <f aca="false">IF(C66=E66, "-", "modifier")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="9" t="s">
         <v>98</v>
       </c>
@@ -1972,6 +2232,10 @@
       <c r="E67" s="8" t="s">
         <v>105</v>
       </c>
+      <c r="G67" s="0" t="str">
+        <f aca="false">IF(C67=E67, "-", "modifier")</f>
+        <v>-</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
@@ -1989,6 +2253,10 @@
       <c r="E68" s="1" t="s">
         <v>108</v>
       </c>
+      <c r="G68" s="0" t="str">
+        <f aca="false">IF(C68=E68, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
@@ -2006,8 +2274,12 @@
       <c r="E69" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G69" s="0" t="str">
+        <f aca="false">IF(C69=E69, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
         <v>5</v>
       </c>
@@ -2019,6 +2291,10 @@
       </c>
       <c r="E70" s="1" t="s">
         <v>111</v>
+      </c>
+      <c r="G70" s="0" t="str">
+        <f aca="false">IF(C70=E70, "-", "modifier")</f>
+        <v>-</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2034,6 +2310,10 @@
       <c r="E71" s="1" t="s">
         <v>112</v>
       </c>
+      <c r="G71" s="0" t="str">
+        <f aca="false">IF(C71=E71, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
@@ -2048,6 +2328,10 @@
       <c r="E72" s="1" t="s">
         <v>113</v>
       </c>
+      <c r="G72" s="0" t="str">
+        <f aca="false">IF(C72=E72, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
@@ -2062,6 +2346,10 @@
       <c r="E73" s="1" t="s">
         <v>114</v>
       </c>
+      <c r="G73" s="0" t="str">
+        <f aca="false">IF(C73=E73, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
@@ -2079,6 +2367,10 @@
       <c r="E74" s="1" t="s">
         <v>116</v>
       </c>
+      <c r="G74" s="0" t="str">
+        <f aca="false">IF(C74=E74, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
@@ -2096,6 +2388,10 @@
       <c r="E75" s="1" t="s">
         <v>118</v>
       </c>
+      <c r="G75" s="0" t="str">
+        <f aca="false">IF(C75=E75, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
@@ -2113,6 +2409,10 @@
       <c r="E76" s="1" t="s">
         <v>120</v>
       </c>
+      <c r="G76" s="0" t="str">
+        <f aca="false">IF(C76=E76, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
@@ -2130,6 +2430,10 @@
       <c r="E77" s="25" t="s">
         <v>122</v>
       </c>
+      <c r="G77" s="0" t="str">
+        <f aca="false">IF(C77=E77, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
@@ -2147,6 +2451,10 @@
       <c r="E78" s="1" t="s">
         <v>124</v>
       </c>
+      <c r="G78" s="0" t="str">
+        <f aca="false">IF(C78=E78, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
@@ -2161,6 +2469,10 @@
       <c r="E79" s="1" t="s">
         <v>125</v>
       </c>
+      <c r="G79" s="0" t="str">
+        <f aca="false">IF(C79=E79, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
@@ -2175,6 +2487,10 @@
       <c r="E80" s="1" t="s">
         <v>126</v>
       </c>
+      <c r="G80" s="0" t="str">
+        <f aca="false">IF(C80=E80, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
@@ -2192,6 +2508,10 @@
       <c r="E81" s="1" t="s">
         <v>128</v>
       </c>
+      <c r="G81" s="0" t="str">
+        <f aca="false">IF(C81=E81, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
@@ -2209,8 +2529,12 @@
       <c r="E82" s="1" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G82" s="0" t="str">
+        <f aca="false">IF(C82=E82, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
         <v>32</v>
       </c>
@@ -2222,6 +2546,10 @@
       </c>
       <c r="E83" s="1" t="s">
         <v>131</v>
+      </c>
+      <c r="G83" s="0" t="str">
+        <f aca="false">IF(C83=E83, "-", "modifier")</f>
+        <v>-</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2240,6 +2568,10 @@
       <c r="E84" s="1" t="s">
         <v>133</v>
       </c>
+      <c r="G84" s="0" t="str">
+        <f aca="false">IF(C84=E84, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="85" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="26" t="s">
@@ -2255,6 +2587,10 @@
         <v>21</v>
       </c>
       <c r="E85" s="26"/>
+      <c r="G85" s="0" t="str">
+        <f aca="false">IF(C85=E85, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="86" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="26" t="s">
@@ -2272,6 +2608,10 @@
       <c r="E86" s="26" t="s">
         <v>136</v>
       </c>
+      <c r="G86" s="0" t="str">
+        <f aca="false">IF(C86=E86, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
@@ -2289,8 +2629,12 @@
       <c r="E87" s="1" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G87" s="0" t="str">
+        <f aca="false">IF(C87=E87, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
         <v>40</v>
       </c>
@@ -2300,11 +2644,18 @@
       <c r="C88" s="1" t="s">
         <v>139</v>
       </c>
+      <c r="D88" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="E88" s="1" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G88" s="0" t="str">
+        <f aca="false">IF(C88=E88, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
         <v>40</v>
       </c>
@@ -2317,8 +2668,12 @@
       <c r="E89" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G89" s="0" t="str">
+        <f aca="false">IF(C89=E89, "-", "modifier")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
         <v>40</v>
       </c>
@@ -2331,8 +2686,12 @@
       <c r="E90" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G90" s="0" t="str">
+        <f aca="false">IF(C90=E90, "-", "modifier")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
         <v>40</v>
       </c>
@@ -2344,6 +2703,10 @@
       </c>
       <c r="E91" s="1" t="s">
         <v>138</v>
+      </c>
+      <c r="G91" s="0" t="str">
+        <f aca="false">IF(C91=E91, "-", "modifier")</f>
+        <v>-</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2362,6 +2725,10 @@
       <c r="E92" s="1" t="s">
         <v>144</v>
       </c>
+      <c r="G92" s="0" t="str">
+        <f aca="false">IF(C92=E92, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
@@ -2379,6 +2746,10 @@
       <c r="E93" s="1" t="s">
         <v>146</v>
       </c>
+      <c r="G93" s="0" t="str">
+        <f aca="false">IF(C93=E93, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
@@ -2396,6 +2767,10 @@
       <c r="E94" s="1" t="s">
         <v>141</v>
       </c>
+      <c r="G94" s="0" t="str">
+        <f aca="false">IF(C94=E94, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
@@ -2413,6 +2788,10 @@
       <c r="E95" s="1" t="s">
         <v>146</v>
       </c>
+      <c r="G95" s="0" t="str">
+        <f aca="false">IF(C95=E95, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
@@ -2430,8 +2809,12 @@
       <c r="E96" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G96" s="0" t="str">
+        <f aca="false">IF(C96=E96, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
         <v>61</v>
       </c>
@@ -2441,8 +2824,15 @@
       <c r="C97" s="1" t="s">
         <v>150</v>
       </c>
+      <c r="D97" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="E97" s="1" t="s">
         <v>151</v>
+      </c>
+      <c r="G97" s="0" t="str">
+        <f aca="false">IF(C97=E97, "-", "modifier")</f>
+        <v>modifier</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2461,6 +2851,10 @@
       <c r="E98" s="1" t="s">
         <v>151</v>
       </c>
+      <c r="G98" s="0" t="str">
+        <f aca="false">IF(C98=E98, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
@@ -2475,8 +2869,12 @@
       <c r="E99" s="1" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G99" s="0" t="str">
+        <f aca="false">IF(C99=E99, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
         <v>69</v>
       </c>
@@ -2488,6 +2886,10 @@
       </c>
       <c r="E100" s="1" t="s">
         <v>154</v>
+      </c>
+      <c r="G100" s="0" t="str">
+        <f aca="false">IF(C100=E100, "-", "modifier")</f>
+        <v>-</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2506,6 +2908,10 @@
       <c r="E101" s="1" t="s">
         <v>156</v>
       </c>
+      <c r="G101" s="0" t="str">
+        <f aca="false">IF(C101=E101, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="102" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="26" t="s">
@@ -2523,6 +2929,10 @@
       <c r="E102" s="26" t="s">
         <v>158</v>
       </c>
+      <c r="G102" s="0" t="str">
+        <f aca="false">IF(C102=E102, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
@@ -2540,6 +2950,10 @@
       <c r="E103" s="1" t="s">
         <v>160</v>
       </c>
+      <c r="G103" s="0" t="str">
+        <f aca="false">IF(C103=E103, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="104" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="26" t="s">
@@ -2557,6 +2971,10 @@
       <c r="E104" s="26" t="s">
         <v>158</v>
       </c>
+      <c r="G104" s="0" t="str">
+        <f aca="false">IF(C104=E104, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
@@ -2574,8 +2992,12 @@
       <c r="E105" s="1" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="106" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G105" s="0" t="str">
+        <f aca="false">IF(C105=E105, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
         <v>69</v>
       </c>
@@ -2587,6 +3009,10 @@
       </c>
       <c r="E106" s="1" t="s">
         <v>164</v>
+      </c>
+      <c r="G106" s="0" t="str">
+        <f aca="false">IF(C106=E106, "-", "modifier")</f>
+        <v>-</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2605,6 +3031,10 @@
       <c r="E107" s="1" t="s">
         <v>166</v>
       </c>
+      <c r="G107" s="0" t="str">
+        <f aca="false">IF(C107=E107, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
@@ -2622,6 +3052,10 @@
       <c r="E108" s="1" t="s">
         <v>167</v>
       </c>
+      <c r="G108" s="0" t="str">
+        <f aca="false">IF(C108=E108, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
@@ -2639,6 +3073,10 @@
       <c r="E109" s="1" t="s">
         <v>122</v>
       </c>
+      <c r="G109" s="0" t="str">
+        <f aca="false">IF(C109=E109, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
@@ -2653,6 +3091,10 @@
       <c r="E110" s="1" t="s">
         <v>168</v>
       </c>
+      <c r="G110" s="0" t="str">
+        <f aca="false">IF(C110=E110, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
@@ -2667,6 +3109,10 @@
       <c r="E111" s="1" t="s">
         <v>169</v>
       </c>
+      <c r="G111" s="0" t="str">
+        <f aca="false">IF(C111=E111, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
@@ -2684,6 +3130,10 @@
       <c r="E112" s="1" t="s">
         <v>170</v>
       </c>
+      <c r="G112" s="0" t="str">
+        <f aca="false">IF(C112=E112, "-", "modifier")</f>
+        <v>-</v>
+      </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
@@ -2701,6 +3151,10 @@
       <c r="E113" s="1" t="s">
         <v>172</v>
       </c>
+      <c r="G113" s="0" t="str">
+        <f aca="false">IF(C113=E113, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
@@ -2718,6 +3172,10 @@
       <c r="E114" s="1" t="s">
         <v>174</v>
       </c>
+      <c r="G114" s="0" t="str">
+        <f aca="false">IF(C114=E114, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
@@ -2735,6 +3193,10 @@
       <c r="E115" s="1" t="s">
         <v>172</v>
       </c>
+      <c r="G115" s="0" t="str">
+        <f aca="false">IF(C115=E115, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="116" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="26" t="s">
@@ -2752,6 +3214,10 @@
       <c r="E116" s="26" t="s">
         <v>177</v>
       </c>
+      <c r="G116" s="0" t="str">
+        <f aca="false">IF(C116=E116, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="117" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
@@ -2766,6 +3232,10 @@
       <c r="E117" s="28" t="s">
         <v>179</v>
       </c>
+      <c r="G117" s="0" t="str">
+        <f aca="false">IF(C117=E117, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="1" t="s">
@@ -2777,6 +3247,10 @@
       <c r="E118" s="1" t="s">
         <v>180</v>
       </c>
+      <c r="G118" s="0" t="str">
+        <f aca="false">IF(C118=E118, "-", "modifier")</f>
+        <v>modifier</v>
+      </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="1" t="s">
@@ -2787,22 +3261,17 @@
       </c>
       <c r="E119" s="1" t="s">
         <v>181</v>
+      </c>
+      <c r="G119" s="0" t="str">
+        <f aca="false">IF(C119=E119, "-", "modifier")</f>
+        <v>modifier</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:E119">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="ajouter"/>
-        <filter val="fusionner"/>
-        <filter val="modifier"/>
-        <filter val="supprimer"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:E119"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>